<commit_message>
cfd dfd event table
</commit_message>
<xml_diff>
--- a/Documentation/SOFTDEV/FINALS/EVENT TABLE.xlsx
+++ b/Documentation/SOFTDEV/FINALS/EVENT TABLE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>EVENT</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>Updated dashboards</t>
+  </si>
+  <si>
+    <t>User views Dashboard</t>
+  </si>
+  <si>
+    <t>Data visualization</t>
+  </si>
+  <si>
+    <t>Visualized data</t>
+  </si>
+  <si>
+    <t>Views Dashboard</t>
   </si>
 </sst>
 </file>
@@ -234,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,16 +257,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -334,16 +349,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G7"/>
   <tableColumns count="7">
     <tableColumn id="1" name="#" dataDxfId="6"/>
     <tableColumn id="2" name="EVENT" dataDxfId="5"/>
     <tableColumn id="3" name="TRIGGER" dataDxfId="4"/>
     <tableColumn id="4" name="SOURCE" dataDxfId="3"/>
     <tableColumn id="5" name="USE CASE" dataDxfId="2"/>
-    <tableColumn id="6" name="RESPONSE" dataDxfId="0"/>
-    <tableColumn id="7" name="DESTINATION" dataDxfId="1"/>
+    <tableColumn id="6" name="RESPONSE" dataDxfId="1"/>
+    <tableColumn id="7" name="DESTINATION" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -796,7 +811,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -944,7 +959,29 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="8" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>